<commit_message>
updating anat stats spreadsheet
</commit_message>
<xml_diff>
--- a/Spreadsheets/PQBC_ABCD_tasks_MRI_stats.xlsx
+++ b/Spreadsheets/PQBC_ABCD_tasks_MRI_stats.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/madeleineseitz/Desktop/thesis/ABCD_Project/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA102620-246F-1341-A223-1A220C83CF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93E339DC-7FCE-C043-AA2E-584A468763EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3680" yWindow="1060" windowWidth="27640" windowHeight="16940" xr2:uid="{C08493BB-222E-F943-98B4-02A4A9154E8F}"/>
+    <workbookView xWindow="3680" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{C08493BB-222E-F943-98B4-02A4A9154E8F}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="anat_task_stats_full_sample" sheetId="1" r:id="rId1"/>
+    <sheet name="refined_LR_anat_task_stats" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t xml:space="preserve">Statistical comparisons of tasks between HR and LR groups (HR defined as having endorsed 4+ PQ-BC items) </t>
   </si>
@@ -108,6 +109,45 @@
   </si>
   <si>
     <t>lmt_scr_num_timed_out</t>
+  </si>
+  <si>
+    <t>Student's t-test</t>
+  </si>
+  <si>
+    <t>SOCIAL INFLUENCE TASK (BEHAVIORAL TASK)--5  of 14 measures significant (see df)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Statistical comparisons of tasks between HR and LR groups (HR defined as having endorsed 4+ PQ-BC items, LR with 0 PQBC endorsement, no family hx of psychiatric illness, matched for ethnicity, sex, and age ) </t>
+  </si>
+  <si>
+    <t>DESIKAN PARCELLATION ANATOMICAL SCANS--74 of 142 measures significant (see df)</t>
+  </si>
+  <si>
+    <t>MID (BEHAVIORAL MEASURES)--0 of 27 measures significant between HR and LR groups)</t>
+  </si>
+  <si>
+    <t>MID (fMRI MEASURES)--SIGNIFICANT MEASURES ONLY (1 of 48 measures significant between HR and LR groups)</t>
+  </si>
+  <si>
+    <t>SST (fMRI MEASURES)--SIGNIFICANT MEASURES ONLY (2 of 98 measures significant between HR and LR groups)</t>
+  </si>
+  <si>
+    <t>tfmri_sacsvis_bscs_crbcxlh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SST (BEHAVIORAL MEASURES)--17 of 29 measures significant (see df) </t>
+  </si>
+  <si>
+    <t>EMOTIONAL N-BACK (fMRI MEASURES)--1 of 90 measures significant (see df)</t>
+  </si>
+  <si>
+    <t>tfmri_nback_all_268</t>
+  </si>
+  <si>
+    <t>GAME OF DICE TASK (BEHAVIORAL TASK) -- 8 of 10 measures significant</t>
+  </si>
+  <si>
+    <t>LITTE MAN TASK (BEHAVIORAL TASK)-- 0 of 4 measures significant</t>
   </si>
 </sst>
 </file>
@@ -185,12 +225,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent6" xfId="1" builtinId="50"/>
@@ -528,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89FB853F-369E-0248-B592-F6E41FAEABEF}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
@@ -772,4 +814,189 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24C405EC-4520-9240-9418-CA75221A86CE}">
+  <dimension ref="A1:C34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" customWidth="1"/>
+    <col min="4" max="4" width="27.5" customWidth="1"/>
+    <col min="5" max="5" width="21.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3">
+        <v>-2.13451635006389</v>
+      </c>
+      <c r="C15" s="3">
+        <v>-2.1716720959236402</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3">
+        <v>3.2915426658321097E-2</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2.9991421236647699E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3">
+        <v>2111</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="3">
+        <v>-2.3413416012142001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1.93083127809986E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" s="3">
+        <v>2085</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="5"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>